<commit_message>
Modified detailedExplanation, add data and results directories
* data and results directories have examples and their results of
execution of the code.
* detailedExplanation has functions to create all possibles schedules
and export them to .xlsx file.
</commit_message>
<xml_diff>
--- a/Data/example_1.xlsx
+++ b/Data/example_1.xlsx
@@ -5,17 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Mi unidad\JupyterNotebooks\Professional Development\universitySchedule\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Mi unidad\JupyterNotebooks\Professional Development\universitySchedule\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B2D5D1C-D79D-4886-BEB8-7FCB4A0D7070}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30BDAA9C-5E73-4520-A3BD-1D6979A6F694}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4680" yWindow="2235" windowWidth="21600" windowHeight="11385" xr2:uid="{6AF61DBB-15FF-4377-B59D-786378A0D84F}"/>
+    <workbookView xWindow="30090" yWindow="1605" windowWidth="21600" windowHeight="11385" activeTab="4" xr2:uid="{6AF61DBB-15FF-4377-B59D-786378A0D84F}"/>
   </bookViews>
   <sheets>
     <sheet name="General Observations" sheetId="3" r:id="rId1"/>
     <sheet name="Organic Chemistry" sheetId="1" r:id="rId2"/>
     <sheet name="Microbiology" sheetId="4" r:id="rId3"/>
+    <sheet name="Mathematics" sheetId="5" r:id="rId4"/>
+    <sheet name="Lenguague" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="58">
   <si>
     <t>option 1</t>
   </si>
@@ -44,127 +46,172 @@
     <t>option 2</t>
   </si>
   <si>
+    <t>Options</t>
+  </si>
+  <si>
+    <t>Days</t>
+  </si>
+  <si>
+    <t>Hours</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>Professor</t>
+  </si>
+  <si>
+    <t>Mo</t>
+  </si>
+  <si>
+    <t>Tu</t>
+  </si>
+  <si>
+    <t>We</t>
+  </si>
+  <si>
+    <t>Th</t>
+  </si>
+  <si>
+    <t>Fr</t>
+  </si>
+  <si>
+    <t>Sa</t>
+  </si>
+  <si>
+    <t>Su</t>
+  </si>
+  <si>
+    <t>Monday</t>
+  </si>
+  <si>
+    <t>Tuesday</t>
+  </si>
+  <si>
+    <t>Wednesday</t>
+  </si>
+  <si>
+    <t>Thursday</t>
+  </si>
+  <si>
+    <t>Friday</t>
+  </si>
+  <si>
+    <t>Saturday</t>
+  </si>
+  <si>
+    <t>Sunday</t>
+  </si>
+  <si>
+    <t>Example:</t>
+  </si>
+  <si>
+    <t>Mo Tu We</t>
+  </si>
+  <si>
+    <t>24 hours format</t>
+  </si>
+  <si>
+    <t>9:30-11:30 15:30-16:00 9:00-10:00</t>
+  </si>
+  <si>
+    <t>Indications to write the days of the different options of the classes</t>
+  </si>
+  <si>
+    <t>Indications to write the hours for start and finish of each class of each day</t>
+  </si>
+  <si>
+    <t>Each day separates by only one white space.</t>
+  </si>
+  <si>
+    <t>It means the class is on Monday, Tuesday and Wednesday</t>
+  </si>
+  <si>
+    <t>It means the class on Monday starts at 9:30 and finishes at 11:30, the same way for  Tuesday and Wednesday in this order.</t>
+  </si>
+  <si>
+    <t>Please use in the hours:</t>
+  </si>
+  <si>
+    <t>Please use in the days:</t>
+  </si>
+  <si>
+    <t>The hours must have the same order of the days</t>
+  </si>
+  <si>
+    <t>To separate hours of each day use only one white space.</t>
+  </si>
+  <si>
+    <t>"-" (minus) symbol to separate start and finish</t>
+  </si>
+  <si>
+    <t>":" symbol to separate hours of the minutes.</t>
+  </si>
+  <si>
+    <t>Advanced example</t>
+  </si>
+  <si>
+    <t>Mo Mo Fr</t>
+  </si>
+  <si>
+    <t>9:30-10:30 13:00-14:00 8:30-9:30</t>
+  </si>
+  <si>
+    <t>Mrs. Bruneto</t>
+  </si>
+  <si>
+    <t>If we have option 1 which have two hours separated on the same day. For example, Chemistry option 1 is on Monday from 9:30 to 10:30 and then from 13:00 to 14:00,  and Friday from 8:30 to 9:30. We need to enter this as two different days as Monday as shown:</t>
+  </si>
+  <si>
+    <t>Please, create a new sheet for each class</t>
+  </si>
+  <si>
+    <t>Mo Mo We</t>
+  </si>
+  <si>
+    <t>8:30-9:30 14:00-15:00 7:30-9:30</t>
+  </si>
+  <si>
+    <t>Mr. Been</t>
+  </si>
+  <si>
+    <t>Tu We Th</t>
+  </si>
+  <si>
+    <t>9:30-11:30 8:30-9:30 9:30-10:30</t>
+  </si>
+  <si>
+    <t>Mr. Solis</t>
+  </si>
+  <si>
+    <t>8:30-9:30</t>
+  </si>
+  <si>
+    <t>Mr. Lee</t>
+  </si>
+  <si>
+    <t>Mr. Gon</t>
+  </si>
+  <si>
+    <t>13:30-14:30</t>
+  </si>
+  <si>
     <t>option 3</t>
   </si>
   <si>
-    <t>Options</t>
-  </si>
-  <si>
-    <t>Days</t>
-  </si>
-  <si>
-    <t>Hours</t>
-  </si>
-  <si>
-    <t>Code</t>
-  </si>
-  <si>
-    <t>Professor</t>
-  </si>
-  <si>
-    <t>Mo</t>
-  </si>
-  <si>
-    <t>Tu</t>
-  </si>
-  <si>
-    <t>We</t>
-  </si>
-  <si>
-    <t>Th</t>
-  </si>
-  <si>
-    <t>Fr</t>
-  </si>
-  <si>
-    <t>Sa</t>
-  </si>
-  <si>
-    <t>Su</t>
-  </si>
-  <si>
-    <t>Monday</t>
-  </si>
-  <si>
-    <t>Tuesday</t>
-  </si>
-  <si>
-    <t>Wednesday</t>
-  </si>
-  <si>
-    <t>Thursday</t>
-  </si>
-  <si>
-    <t>Friday</t>
-  </si>
-  <si>
-    <t>Saturday</t>
-  </si>
-  <si>
-    <t>Sunday</t>
-  </si>
-  <si>
-    <t>Example:</t>
-  </si>
-  <si>
-    <t>Mo Tu We</t>
-  </si>
-  <si>
-    <t>24 hours format</t>
-  </si>
-  <si>
-    <t>9:30-11:30 15:30-16:00 9:00-10:00</t>
-  </si>
-  <si>
-    <t>Indications to write the days of the different options of the classes</t>
-  </si>
-  <si>
-    <t>Indications to write the hours for start and finish of each class of each day</t>
-  </si>
-  <si>
-    <t>Each day separates by only one white space.</t>
-  </si>
-  <si>
-    <t>It means the class is on Monday, Tuesday and Wednesday</t>
-  </si>
-  <si>
-    <t>It means the class on Monday starts at 9:30 and finishes at 11:30, the same way for  Tuesday and Wednesday in this order.</t>
-  </si>
-  <si>
-    <t>Please use in the hours:</t>
-  </si>
-  <si>
-    <t>Please use in the days:</t>
-  </si>
-  <si>
-    <t>The hours must have the same order of the days</t>
-  </si>
-  <si>
-    <t>To separate hours of each day use only one white space.</t>
-  </si>
-  <si>
-    <t>"-" (minus) symbol to separate start and finish</t>
-  </si>
-  <si>
-    <t>":" symbol to separate hours of the minutes.</t>
-  </si>
-  <si>
-    <t>Advanced example</t>
-  </si>
-  <si>
-    <t>Mo Mo Fr</t>
-  </si>
-  <si>
-    <t>9:30-10:30 13:00-14:00 8:30-9:30</t>
-  </si>
-  <si>
-    <t>Mrs. Bruneto</t>
-  </si>
-  <si>
-    <t>If we have option 1 which have two hours separated on the same day. For example, Chemistry option 1 is on Monday from 9:30 to 10:30 and then from 13:00 to 14:00,  and Friday from 8:30 to 9:30. We need to enter this as two different days as Monday as shown:</t>
-  </si>
-  <si>
-    <t>Please, create a new sheet for each class</t>
+    <t>12:00-13:00</t>
+  </si>
+  <si>
+    <t>11:00-12:00</t>
+  </si>
+  <si>
+    <t>Mr. Org</t>
+  </si>
+  <si>
+    <t>9:00-11:00</t>
+  </si>
+  <si>
+    <t>12:30-13:30</t>
   </si>
 </sst>
 </file>
@@ -269,17 +316,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -287,16 +326,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -613,8 +660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63DD08DA-CA54-4BEE-86D1-70ADD9A13406}">
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -623,14 +670,14 @@
     <col min="2" max="2" width="22" customWidth="1"/>
     <col min="3" max="3" width="29.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.42578125" customWidth="1"/>
-    <col min="7" max="7" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
@@ -638,38 +685,38 @@
     </row>
     <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>29</v>
+        <v>8</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>28</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F4" s="10"/>
       <c r="G4" s="10"/>
@@ -678,84 +725,84 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="11"/>
-      <c r="E5" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
+        <v>9</v>
+      </c>
+      <c r="C5" s="13"/>
+      <c r="E5" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="11"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
+        <v>10</v>
+      </c>
+      <c r="C6" s="13"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="11"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
+        <v>11</v>
+      </c>
+      <c r="C7" s="13"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="11"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
+        <v>12</v>
+      </c>
+      <c r="C8" s="13"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="11"/>
+        <v>13</v>
+      </c>
+      <c r="C9" s="13"/>
       <c r="E9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="G9" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="H9" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="I9" s="3" t="s">
         <v>6</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -763,21 +810,21 @@
         <v>0</v>
       </c>
       <c r="F10" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G10" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>39</v>
       </c>
       <c r="H10" s="2">
         <v>2504</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B11" s="10"/>
       <c r="C11" s="10"/>
@@ -785,67 +832,73 @@
     </row>
     <row r="12" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B12" s="10"/>
       <c r="C12" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E12" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="16"/>
+        <v>41</v>
+      </c>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="18"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="11"/>
+      <c r="C13" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="13"/>
-      <c r="C13" s="6" t="s">
-        <v>25</v>
-      </c>
     </row>
     <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="11"/>
+      <c r="C14" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="G14" s="9"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="14"/>
+      <c r="C15" s="13"/>
+    </row>
+    <row r="16" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="13"/>
-      <c r="C14" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="G14" s="18"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="15" t="s">
+      <c r="B16" s="16"/>
+      <c r="C16" s="13"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="16"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="13"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="B15" s="15"/>
-      <c r="C15" s="11"/>
-    </row>
-    <row r="16" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="B16" s="12"/>
-      <c r="C16" s="11"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="12"/>
-      <c r="B17" s="12"/>
-      <c r="C17" s="11"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="B18" s="14"/>
-      <c r="C18" s="11"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="E5:I8"/>
+    <mergeCell ref="E4:I4"/>
+    <mergeCell ref="C14:C18"/>
+    <mergeCell ref="A16:B17"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="E12:I12"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A11:C11"/>
     <mergeCell ref="A18:B18"/>
@@ -853,12 +906,6 @@
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>
-    <mergeCell ref="E5:I8"/>
-    <mergeCell ref="E4:I4"/>
-    <mergeCell ref="C14:C18"/>
-    <mergeCell ref="A16:B17"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="E12:I12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -867,10 +914,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB41DE9C-28CB-4A32-A262-A64A54FCC521}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -883,34 +930,53 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="C1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="D1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="7" t="s">
         <v>6</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
+      <c r="B2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2">
+        <v>1718</v>
+      </c>
+      <c r="E2" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
+      <c r="B3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3">
+        <v>1550</v>
+      </c>
+      <c r="E3" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -920,7 +986,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D597654-FA0E-40ED-AB83-0333807273CE}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C23" sqref="C23"/>
@@ -936,40 +1002,218 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="C1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="D1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="7" t="s">
         <v>6</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2">
+        <v>1715</v>
+      </c>
+      <c r="E2" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3">
+        <v>1875</v>
+      </c>
+      <c r="E3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E4" s="8"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C16" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B869205E-8F2C-47C4-B9F9-FFA2547864AD}">
+  <dimension ref="A1:E16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="3" max="3" width="48.7109375" customWidth="1"/>
+    <col min="5" max="5" width="30.7109375" customWidth="1"/>
+    <col min="6" max="6" width="25.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2">
+        <v>1715</v>
+      </c>
+      <c r="E2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3">
+        <v>1875</v>
+      </c>
+      <c r="E3" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C17" s="8"/>
+        <v>52</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4">
+        <v>1965</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C16" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8486D357-1B34-41E2-9E67-8600BEDFDDD6}">
+  <dimension ref="A1:E15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="3" max="3" width="48.7109375" customWidth="1"/>
+    <col min="5" max="5" width="30.7109375" customWidth="1"/>
+    <col min="6" max="6" width="25.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2">
+        <v>1715</v>
+      </c>
+      <c r="E2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E3" s="8"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C15" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>